<commit_message>
Numerous Updates: 1. Coloured markers according to route. Only start and end points in red. 2. The sidebar now displays the distance 3. Cleaned up unused code.
</commit_message>
<xml_diff>
--- a/Dataset/ETS Train.xlsx
+++ b/Dataset/ETS Train.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JasonX\PycharmProjects\Algo-Assignment\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F41C279-6623-429E-A7A9-C54A193D4EFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94248F1-B7BA-4E20-A215-458DFDBFB9C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3DFF64DC-D989-47BF-B042-34AAD9B60226}"/>
   </bookViews>
@@ -47,69 +47,39 @@
     <t>UTARA</t>
   </si>
   <si>
-    <t>TANJONG MALIM</t>
-  </si>
-  <si>
     <t>STESEN KTM TANJUNG MALIM,  35900 TANJUNG MALIM</t>
   </si>
   <si>
-    <t>KUALA KUBU BAHRU</t>
-  </si>
-  <si>
     <t xml:space="preserve">STESEN KERETAPI KUALA KUBU BHARU, KUALA KUBU BHARU, SELANGOR, </t>
   </si>
   <si>
-    <t>BATANG KALI</t>
-  </si>
-  <si>
     <t>3.468380</t>
   </si>
   <si>
     <t>STESEN KTM KOMUTER BATANG KALI, 44200 BATANG KALI, SELANGOR</t>
   </si>
   <si>
-    <t>RAWANG</t>
-  </si>
-  <si>
     <t xml:space="preserve">STESEN KERETAPI RAWANG, 41300 RAWANG, SELANGOR, </t>
   </si>
   <si>
-    <t>SUNGAI BULOH</t>
-  </si>
-  <si>
     <t>STESEN KERETAPI SUNGAI BULOH, LOT 3, JALAN KUALA SELANGOR, 47000 SUNGAI BULOH</t>
   </si>
   <si>
     <t>WILAYAH PERSEKUTUAN</t>
   </si>
   <si>
-    <t>KEPONG SENTRAL</t>
-  </si>
-  <si>
     <t>STESEN KTM KOMUTER KEPONG SENTRAL, 52200 SUNGAI BULOH, SELANGOR</t>
   </si>
   <si>
-    <t>KUALA LUMPUR</t>
-  </si>
-  <si>
     <t>KUALA LUMPUR RAILWAY,  JALAN SULTAN HISHAMUDDIN,  50621 KUALA LUMPUR</t>
   </si>
   <si>
-    <t>KL SENTRAL</t>
-  </si>
-  <si>
     <t>KUALA LUMPUR SENTRAL,  50470 KUALA LUMPUR</t>
   </si>
   <si>
-    <t>BANDAR TASEK SELATAN</t>
-  </si>
-  <si>
     <t>STESEN KTMB BANDAR TASIK SELATAN SELATAN, JALAN LINGKARAN TENGAH 2, KUALA LUMPUR</t>
   </si>
   <si>
-    <t xml:space="preserve">KAJANG </t>
-  </si>
-  <si>
     <t>STESEN KTM KOMUTER KAJANG, 43000 KAJANG, SELANGOR</t>
   </si>
   <si>
@@ -119,18 +89,12 @@
     <t>SELATAN</t>
   </si>
   <si>
-    <t>SEREMBAN</t>
-  </si>
-  <si>
     <t>KTM KOMUTER,  BANDAR SEREMBAN, 70300 SEREMBAN</t>
   </si>
   <si>
     <t>MELAKA</t>
   </si>
   <si>
-    <t>PULAU SEBANG/TAMPIN</t>
-  </si>
-  <si>
     <t>2.463710</t>
   </si>
   <si>
@@ -158,166 +122,202 @@
     <t>STATE</t>
   </si>
   <si>
+    <t>PERLIS</t>
+  </si>
+  <si>
+    <t>STESEN KERETAPI PADANG BESAR 02100 PADANG BESAR</t>
+  </si>
+  <si>
+    <t>STESEN KERETAPI ARAU, JALAN STESYEN, 02600, ARAU, PERLIS</t>
+  </si>
+  <si>
+    <t>KEDAH</t>
+  </si>
+  <si>
+    <t>STESEN ANAK BUKIT, 05150 ALOR SETAR, KEDAH</t>
+  </si>
+  <si>
+    <t>STESEN KTM ALOR SETAR, JALAN KOLAM AIR, ALOR MALAI  05200 ALOR SETAR</t>
+  </si>
+  <si>
+    <t>STESEN SEMENTARA KTMB, KAMPUNG PULAU CENGAL, 08300 GURUN.</t>
+  </si>
+  <si>
+    <t>STESYEN KTM,  JLN IBRAHIM, 8000,  SUNGAI PETANI</t>
+  </si>
+  <si>
+    <t>PULAU PINANG</t>
+  </si>
+  <si>
+    <t>STESEN KTM TASEK GELUGOR, 13100 TASEK GELUGOR</t>
+  </si>
+  <si>
+    <t>STESEN KTM BUKIT MERTAJAM, 2916,  JALAN PADANG LALANG,  14000 BUKIT MERTAJAM</t>
+  </si>
+  <si>
+    <t>STESEN KERETAPI KAMPUNG PERMATANG TOK MAMAT,  34200 PARIT BUNTAR</t>
+  </si>
+  <si>
+    <t>STESEN BAGAN SERAI, 34300 BAGAN SERAI, PERAK</t>
+  </si>
+  <si>
+    <t>TAIPING RAILWAY,  JALAN STESEN,  34000 TAIPING</t>
+  </si>
+  <si>
+    <t>STESEN KTM PADANG RENGAS, 33700 PADANG RENGAS, PERAK</t>
+  </si>
+  <si>
+    <t>STESEN KERETAPI KUALA KANGSAR, JALAN TUN RAZAK,  33000 KUALA KANGSAR</t>
+  </si>
+  <si>
+    <t>STESEN KERETAPI SUNGAI SIPUT, 31100 SUNGAI SIPUT UTARA, PERAK, MALAYSIA</t>
+  </si>
+  <si>
+    <t>101.073330</t>
+  </si>
+  <si>
+    <t>STESEN KERETAPI IPOH,  JALAN PANGLIMA BUKIT GANTANG WAHAB,  30000 IPOH</t>
+  </si>
+  <si>
+    <t>101.049300</t>
+  </si>
+  <si>
+    <t>STESEN BATU GAJAH, MUKIM, KAMPUNG PISANG, 31000 BATU GAJAH, PERAK</t>
+  </si>
+  <si>
+    <t>STESEN KERETAPI KAMPAR, JALAN STESEN, 31900 KAMPAR, PERAK, MALAYSIA.</t>
+  </si>
+  <si>
+    <t>STESEN KERETAPI SUNGKAI, 35600 SUNGKAI, PERAK, MALAYSIA.</t>
+  </si>
+  <si>
+    <t>STESEN KERETAPI SLIM RIVER, JALAN STESEN, 35800 SLIM RIVER, PERAK, MALAYSIA.</t>
+  </si>
+  <si>
+    <t>STESEN KTM BEHRANG, 35950 BEHRANG STESEN, PERAK</t>
+  </si>
+  <si>
+    <t>STESEN KTM BATANG MELAKA, 77500 BATANG MELAKA, MELAKA</t>
+  </si>
+  <si>
+    <t>STESEN KTM GEMAS, KAWASAN INDUSTRI GEMAS,  73400 GEMAS</t>
+  </si>
+  <si>
+    <t>STESEN KERETAPI BUTTERWORTH, JALAN BAGAN DALAM, 12000 BUTTERWORTH</t>
+  </si>
+  <si>
+    <t>ETS MAIN</t>
+  </si>
+  <si>
+    <t>ETS ALT</t>
+  </si>
+  <si>
+    <t>Stesen Keretapi Padang Besar</t>
+  </si>
+  <si>
+    <t>Stesen Keretapi Arau</t>
+  </si>
+  <si>
+    <t>Stesen Anak Bukit</t>
+  </si>
+  <si>
+    <t>Stesen Keretapi Kampung Permatang Tok Mamat</t>
+  </si>
+  <si>
+    <t>Stesen Bagan Serai</t>
+  </si>
+  <si>
+    <t>Taiping Railway</t>
+  </si>
+  <si>
+    <t>Stesen Keretapi Kuala Kangsar</t>
+  </si>
+  <si>
+    <t>Stesen Keretapi Sungai Siput</t>
+  </si>
+  <si>
+    <t>Stesen Keretapi Ipoh</t>
+  </si>
+  <si>
+    <t>Stesen Batu Gajah</t>
+  </si>
+  <si>
+    <t>Stesen Keretapi Kampar</t>
+  </si>
+  <si>
+    <t>Stesen Keretapi Sungkai</t>
+  </si>
+  <si>
+    <t>Stesen Keretapi Slim River</t>
+  </si>
+  <si>
+    <t>Stesen Keretapi Kuala Kubu Bharu</t>
+  </si>
+  <si>
+    <t>Stesen Keretapi Rawang</t>
+  </si>
+  <si>
+    <t>Stesen Keretapi Sungai Buloh</t>
+  </si>
+  <si>
+    <t>Kuala Lumpur Railway</t>
+  </si>
+  <si>
+    <t>Kuala Lumpur Sentral</t>
+  </si>
+  <si>
+    <t>Stesen Keretapi Butterworth</t>
+  </si>
+  <si>
+    <t>Stesen KTM Alor Setar</t>
+  </si>
+  <si>
+    <t>Stesen KTM Tasek Gelugor</t>
+  </si>
+  <si>
+    <t>Stesen KTM Bukit Mertajam</t>
+  </si>
+  <si>
+    <t>Stesen KTM Padang Rengas</t>
+  </si>
+  <si>
+    <t>Stesen KTM Behrang</t>
+  </si>
+  <si>
+    <t>Stesen KTM Tanjung Malim</t>
+  </si>
+  <si>
+    <t>Stesen KTM Komuter Batang Kali</t>
+  </si>
+  <si>
+    <t>Stesen KTM Komuter Kepong Sentral</t>
+  </si>
+  <si>
+    <t>Stesen KTM Komuter Kajang</t>
+  </si>
+  <si>
+    <t>KTM Komuter Seremban</t>
+  </si>
+  <si>
+    <t>Stesen KTM Pulau Sebang</t>
+  </si>
+  <si>
+    <t>Stesen KTM Batang Melaka</t>
+  </si>
+  <si>
+    <t>Stesen KTM Gemas</t>
+  </si>
+  <si>
+    <t>Stesen KTMB Bandar Tasik Selatan Selatan</t>
+  </si>
+  <si>
+    <t>Stesen Sementara KTMB Gurun</t>
+  </si>
+  <si>
+    <t>Stesyen KTM Sungai Petani</t>
+  </si>
+  <si>
     <t>STATION</t>
-  </si>
-  <si>
-    <t>PERLIS</t>
-  </si>
-  <si>
-    <t>PADANG BESAR</t>
-  </si>
-  <si>
-    <t>STESEN KERETAPI PADANG BESAR 02100 PADANG BESAR</t>
-  </si>
-  <si>
-    <t>ARAU</t>
-  </si>
-  <si>
-    <t>STESEN KERETAPI ARAU, JALAN STESYEN, 02600, ARAU, PERLIS</t>
-  </si>
-  <si>
-    <t>KEDAH</t>
-  </si>
-  <si>
-    <t>ANAK BUKIT</t>
-  </si>
-  <si>
-    <t>STESEN ANAK BUKIT, 05150 ALOR SETAR, KEDAH</t>
-  </si>
-  <si>
-    <t>ALOR SETAR</t>
-  </si>
-  <si>
-    <t>STESEN KTM ALOR SETAR, JALAN KOLAM AIR, ALOR MALAI  05200 ALOR SETAR</t>
-  </si>
-  <si>
-    <t>GURUN</t>
-  </si>
-  <si>
-    <t>STESEN SEMENTARA KTMB, KAMPUNG PULAU CENGAL, 08300 GURUN.</t>
-  </si>
-  <si>
-    <t>SUNGAI PETANI</t>
-  </si>
-  <si>
-    <t>STESYEN KTM,  JLN IBRAHIM, 8000,  SUNGAI PETANI</t>
-  </si>
-  <si>
-    <t>PULAU PINANG</t>
-  </si>
-  <si>
-    <t>TASEK GELUGOR</t>
-  </si>
-  <si>
-    <t>STESEN KTM TASEK GELUGOR, 13100 TASEK GELUGOR</t>
-  </si>
-  <si>
-    <t>BUKIT MERTAJAM</t>
-  </si>
-  <si>
-    <t>STESEN KTM BUKIT MERTAJAM, 2916,  JALAN PADANG LALANG,  14000 BUKIT MERTAJAM</t>
-  </si>
-  <si>
-    <t>PARIT BUNTAR</t>
-  </si>
-  <si>
-    <t>STESEN KERETAPI KAMPUNG PERMATANG TOK MAMAT,  34200 PARIT BUNTAR</t>
-  </si>
-  <si>
-    <t>BAGAN SERAI</t>
-  </si>
-  <si>
-    <t>STESEN BAGAN SERAI, 34300 BAGAN SERAI, PERAK</t>
-  </si>
-  <si>
-    <t>TAIPING</t>
-  </si>
-  <si>
-    <t>TAIPING RAILWAY,  JALAN STESEN,  34000 TAIPING</t>
-  </si>
-  <si>
-    <t>PADANG RENGAS</t>
-  </si>
-  <si>
-    <t>STESEN KTM PADANG RENGAS, 33700 PADANG RENGAS, PERAK</t>
-  </si>
-  <si>
-    <t>KUALA KANGSAR</t>
-  </si>
-  <si>
-    <t>STESEN KERETAPI KUALA KANGSAR, JALAN TUN RAZAK,  33000 KUALA KANGSAR</t>
-  </si>
-  <si>
-    <t>SUNGAI SIPUT</t>
-  </si>
-  <si>
-    <t>STESEN KERETAPI SUNGAI SIPUT, 31100 SUNGAI SIPUT UTARA, PERAK, MALAYSIA</t>
-  </si>
-  <si>
-    <t>IPOH</t>
-  </si>
-  <si>
-    <t>101.073330</t>
-  </si>
-  <si>
-    <t>STESEN KERETAPI IPOH,  JALAN PANGLIMA BUKIT GANTANG WAHAB,  30000 IPOH</t>
-  </si>
-  <si>
-    <t>BATU GAJAH</t>
-  </si>
-  <si>
-    <t>101.049300</t>
-  </si>
-  <si>
-    <t>STESEN BATU GAJAH, MUKIM, KAMPUNG PISANG, 31000 BATU GAJAH, PERAK</t>
-  </si>
-  <si>
-    <t>KAMPAR</t>
-  </si>
-  <si>
-    <t>STESEN KERETAPI KAMPAR, JALAN STESEN, 31900 KAMPAR, PERAK, MALAYSIA.</t>
-  </si>
-  <si>
-    <t>SUNGKAI</t>
-  </si>
-  <si>
-    <t>STESEN KERETAPI SUNGKAI, 35600 SUNGKAI, PERAK, MALAYSIA.</t>
-  </si>
-  <si>
-    <t>SLIM RIVER</t>
-  </si>
-  <si>
-    <t>STESEN KERETAPI SLIM RIVER, JALAN STESEN, 35800 SLIM RIVER, PERAK, MALAYSIA.</t>
-  </si>
-  <si>
-    <t>BEHRANG</t>
-  </si>
-  <si>
-    <t>STESEN KTM BEHRANG, 35950 BEHRANG STESEN, PERAK</t>
-  </si>
-  <si>
-    <t>BATANG MELAKA</t>
-  </si>
-  <si>
-    <t>STESEN KTM BATANG MELAKA, 77500 BATANG MELAKA, MELAKA</t>
-  </si>
-  <si>
-    <t>GEMAS</t>
-  </si>
-  <si>
-    <t>STESEN KTM GEMAS, KAWASAN INDUSTRI GEMAS,  73400 GEMAS</t>
-  </si>
-  <si>
-    <t>BUTTERWORTH</t>
-  </si>
-  <si>
-    <t>STESEN KERETAPI BUTTERWORTH, JALAN BAGAN DALAM, 12000 BUTTERWORTH</t>
-  </si>
-  <si>
-    <t>ETS MAIN</t>
-  </si>
-  <si>
-    <t>ETS ALT</t>
   </si>
 </sst>
 </file>
@@ -733,7 +733,7 @@
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="I2" sqref="I2:I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -749,39 +749,39 @@
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>41</v>
+        <v>94</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="D2" s="5">
         <v>6.6622050000000002</v>
@@ -790,24 +790,24 @@
         <v>100.319514</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="D3" s="5">
         <v>6.4319519999999999</v>
@@ -816,24 +816,24 @@
         <v>100.269002</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="D4" s="5">
         <v>6.183395</v>
@@ -842,24 +842,24 @@
         <v>100.37487400000001</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="D5" s="5">
         <v>6.1131359999999999</v>
@@ -868,24 +868,24 @@
         <v>100.369291</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>52</v>
+        <v>92</v>
       </c>
       <c r="D6" s="5">
         <v>5.8242909999999997</v>
@@ -894,24 +894,24 @@
         <v>100.477451</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>54</v>
+        <v>93</v>
       </c>
       <c r="D7" s="5">
         <v>5.6429780000000003</v>
@@ -920,24 +920,24 @@
         <v>100.489755</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="D8" s="5">
         <v>5.4821749999999998</v>
@@ -946,24 +946,24 @@
         <v>100.497955</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="D9" s="5">
         <v>5.3659980000000003</v>
@@ -972,13 +972,13 @@
         <v>100.447993</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -989,7 +989,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D10" s="5">
         <v>5.1305709999999998</v>
@@ -998,13 +998,13 @@
         <v>100.486575</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -1024,13 +1024,13 @@
         <v>100.527197</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -1041,7 +1041,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D12" s="5">
         <v>4.8520589999999997</v>
@@ -1050,13 +1050,13 @@
         <v>100.731489</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -1067,7 +1067,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="D13" s="5">
         <v>4.7779319999999998</v>
@@ -1076,13 +1076,13 @@
         <v>100.85742399999999</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -1093,7 +1093,7 @@
         <v>3</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D14" s="5">
         <v>4.7765240000000002</v>
@@ -1102,13 +1102,13 @@
         <v>100.93260100000001</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -1119,7 +1119,7 @@
         <v>3</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D15" s="5">
         <v>4.8187569999999997</v>
@@ -1128,13 +1128,13 @@
         <v>101.07126100000001</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -1145,22 +1145,22 @@
         <v>3</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D16" s="5">
         <v>4.5975260000000002</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -1171,22 +1171,22 @@
         <v>3</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D17" s="5">
         <v>4.4598940000000002</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -1197,7 +1197,7 @@
         <v>3</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="D18" s="5">
         <v>4.3027870000000004</v>
@@ -1206,13 +1206,13 @@
         <v>101.15351200000001</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -1223,22 +1223,22 @@
         <v>3</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D19" s="5">
         <v>4.5975260000000002</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -1249,7 +1249,7 @@
         <v>3</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="D20" s="5">
         <v>3.827134</v>
@@ -1258,13 +1258,13 @@
         <v>101.402164</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -1275,7 +1275,7 @@
         <v>3</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D21" s="5">
         <v>3.7454770000000002</v>
@@ -1284,13 +1284,13 @@
         <v>101.450007</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>86</v>
+        <v>53</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -1301,7 +1301,7 @@
         <v>3</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>4</v>
+        <v>83</v>
       </c>
       <c r="D22" s="5">
         <v>3.6851419999999999</v>
@@ -1310,13 +1310,13 @@
         <v>101.518165</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -1327,7 +1327,7 @@
         <v>1</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>6</v>
+        <v>72</v>
       </c>
       <c r="D23" s="5">
         <v>3.5532149999999998</v>
@@ -1336,13 +1336,13 @@
         <v>101.639591</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -1353,22 +1353,22 @@
         <v>1</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>8</v>
+        <v>84</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E24" s="5">
         <v>101.637759</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -1379,7 +1379,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D25" s="5">
         <v>3.3189549999999999</v>
@@ -1388,13 +1388,13 @@
         <v>101.575012</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -1404,8 +1404,8 @@
       <c r="B26" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>13</v>
+      <c r="C26" s="6" t="s">
+        <v>74</v>
       </c>
       <c r="D26" s="5">
         <v>3.206356</v>
@@ -1414,24 +1414,24 @@
         <v>101.580128</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>16</v>
+        <v>85</v>
       </c>
       <c r="D27" s="5">
         <v>3.2067543999999999</v>
@@ -1440,24 +1440,24 @@
         <v>101.627081</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>18</v>
+        <v>75</v>
       </c>
       <c r="D28" s="5">
         <v>3.1394440000000001</v>
@@ -1466,24 +1466,24 @@
         <v>101.693333</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="D29" s="5">
         <v>3.1341670000000001</v>
@@ -1492,24 +1492,24 @@
         <v>101.686111</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>22</v>
+        <v>91</v>
       </c>
       <c r="D30" s="5">
         <v>3.0762290000000001</v>
@@ -1518,13 +1518,13 @@
         <v>101.711119</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
@@ -1535,7 +1535,7 @@
         <v>1</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>24</v>
+        <v>86</v>
       </c>
       <c r="D31" s="5">
         <v>2.983222</v>
@@ -1544,24 +1544,24 @@
         <v>101.79066899999999</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>28</v>
+        <v>87</v>
       </c>
       <c r="D32" s="5">
         <v>2.7191689999999999</v>
@@ -1570,50 +1570,50 @@
         <v>101.940792</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>31</v>
+        <v>88</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="E33" s="5">
         <v>102.226269</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D34" s="5">
         <v>2.4737429999999998</v>
@@ -1622,24 +1622,24 @@
         <v>102.41569800000001</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D35" s="5">
         <v>2.5796060000000001</v>
@@ -1648,24 +1648,24 @@
         <v>102.611682</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="D36" s="5">
         <v>5.3659980000000003</v>
@@ -1674,24 +1674,24 @@
         <v>100.447993</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D37" s="5">
         <v>5.3933429999999998</v>
@@ -1700,13 +1700,13 @@
         <v>100.366201</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>